<commit_message>
Correção home e mostrar projetos
Atualização dos sql da home e mostraProjetos
</commit_message>
<xml_diff>
--- a/Documentação/Estimativa_de_tamanho.xlsx
+++ b/Documentação/Estimativa_de_tamanho.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\trabalhofinal\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pfcoletivo\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Requisitos</t>
   </si>
@@ -162,12 +162,18 @@
   </si>
   <si>
     <t>Colunas1</t>
+  </si>
+  <si>
+    <t>Implementação</t>
+  </si>
+  <si>
+    <t>Teste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -212,7 +218,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -226,15 +239,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F37" totalsRowShown="0">
-  <autoFilter ref="A1:F37"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:H37" totalsRowShown="0">
+  <autoFilter ref="A1:H37"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Requisitos"/>
     <tableColumn id="2" name="Peso RF"/>
     <tableColumn id="3" name="Peso ator"/>
     <tableColumn id="4" name="TAMANHO"/>
     <tableColumn id="5" name="TAMANHO GLOBAL"/>
     <tableColumn id="6" name="Colunas1"/>
+    <tableColumn id="7" name="Implementação" dataDxfId="1">
+      <calculatedColumnFormula>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Teste" dataDxfId="0">
+      <calculatedColumnFormula>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -549,21 +568,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,8 +601,14 @@
       <c r="F1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -598,8 +623,16 @@
         <v>9.6300000000000008</v>
       </c>
       <c r="E2">
-        <f>D2*3</f>
-        <v>28.89</v>
+        <f>D2*1.5</f>
+        <v>14.445</v>
+      </c>
+      <c r="G2">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H2">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>
@@ -608,7 +641,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -623,8 +656,16 @@
         <v>19.260000000000002</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E36" si="1">D3*3</f>
-        <v>57.78</v>
+        <f t="shared" ref="E3:E36" si="1">D3*1.5</f>
+        <v>28.89</v>
+      </c>
+      <c r="G3">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>14.445</v>
+      </c>
+      <c r="H3">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>2.8890000000000002</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
@@ -633,7 +674,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -649,7 +690,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>28.89</v>
+        <v>14.445</v>
+      </c>
+      <c r="G4">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H4">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -658,7 +707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -674,10 +723,18 @@
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G5">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H5">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -693,10 +750,18 @@
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G6">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H6">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -712,10 +777,18 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G7">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H7">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -731,10 +804,18 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>28.89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>14.445</v>
+      </c>
+      <c r="G8">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H8">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -750,10 +831,18 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G9">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H9">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -769,13 +858,21 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>14.445</v>
+        <v>7.2225000000000001</v>
       </c>
       <c r="F10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H10">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -791,10 +888,18 @@
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G11">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H11">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -810,10 +915,18 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G12">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H12">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -829,10 +942,18 @@
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G13">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H13">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -848,10 +969,18 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>43.335000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>21.6675</v>
+      </c>
+      <c r="G14">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>10.83375</v>
+      </c>
+      <c r="H14">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>2.16675</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -867,10 +996,18 @@
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G15">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H15">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -886,10 +1023,18 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>28.89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14.445</v>
+      </c>
+      <c r="G16">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H16">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -905,10 +1050,18 @@
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G17">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H17">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -924,10 +1077,18 @@
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G18">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H18">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -943,10 +1104,18 @@
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>28.89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14.445</v>
+      </c>
+      <c r="G19">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H19">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -962,10 +1131,18 @@
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G20">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H20">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -981,10 +1158,18 @@
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G21">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H21">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1000,10 +1185,18 @@
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G22">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H22">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1019,10 +1212,18 @@
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G23">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H23">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1038,10 +1239,18 @@
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G24">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H24">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1057,10 +1266,18 @@
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G25">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H25">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1076,10 +1293,18 @@
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G26">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H26">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1095,10 +1320,18 @@
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G27">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H27">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1114,10 +1347,18 @@
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>28.89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14.445</v>
+      </c>
+      <c r="G28">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H28">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1133,10 +1374,18 @@
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>28.89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14.445</v>
+      </c>
+      <c r="G29">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H29">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1152,10 +1401,18 @@
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G30">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H30">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1171,10 +1428,18 @@
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G31">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H31">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1190,10 +1455,18 @@
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G32">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H32">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1209,10 +1482,18 @@
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>28.89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14.445</v>
+      </c>
+      <c r="G33">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H33">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1228,10 +1509,18 @@
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
-        <v>28.89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14.445</v>
+      </c>
+      <c r="G34">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="H34">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>1.4445000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1247,10 +1536,18 @@
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G35">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H35">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1266,10 +1563,18 @@
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
-        <v>14.445</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2225000000000001</v>
+      </c>
+      <c r="G36">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>3.6112500000000001</v>
+      </c>
+      <c r="H36">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>0.72225000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -1279,7 +1584,15 @@
       </c>
       <c r="E37">
         <f>SUM(E2:E36)</f>
-        <v>707.80500000000006</v>
+        <v>353.90250000000003</v>
+      </c>
+      <c r="G37">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.5</f>
+        <v>176.95125000000002</v>
+      </c>
+      <c r="H37">
+        <f>Tabela1[[#This Row],[TAMANHO GLOBAL]]*0.1</f>
+        <v>35.390250000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização cronograma e correção de bug
Atualização cronograma e correção de bugs na home e buscar projeto
candidato
</commit_message>
<xml_diff>
--- a/Documentação/Estimativa_de_tamanho.xlsx
+++ b/Documentação/Estimativa_de_tamanho.xlsx
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>